<commit_message>
Add comparison with TAVRIDA
</commit_message>
<xml_diff>
--- a/ДанныеПоСетям/Кашино/dataTP.xlsx
+++ b/ДанныеПоСетям/Кашино/dataTP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="11">
   <si>
     <t>№ линии</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>=СЧЁТЗ(C3:C92)</t>
+  </si>
+  <si>
+    <t>7494</t>
+  </si>
+  <si>
+    <t>Кол-во линий</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -165,6 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -445,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C92"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,14 +463,15 @@
     <col min="3" max="3" width="8.7265625" style="7"/>
     <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -476,8 +484,11 @@
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" s="13">
         <v>1</v>
       </c>
@@ -490,8 +501,11 @@
       <c r="E3" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="13">
         <v>2</v>
       </c>
@@ -504,8 +518,11 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" s="13">
         <v>3</v>
       </c>
@@ -518,8 +535,11 @@
       <c r="E5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" s="13">
         <v>4</v>
       </c>
@@ -532,8 +552,11 @@
       <c r="E6" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" s="13">
         <v>5</v>
       </c>
@@ -546,8 +569,11 @@
       <c r="E7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
         <v>6</v>
       </c>
@@ -560,8 +586,11 @@
       <c r="E8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="13">
         <v>7</v>
       </c>
@@ -574,8 +603,11 @@
       <c r="E9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="13">
         <v>8</v>
       </c>
@@ -588,8 +620,11 @@
       <c r="E10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <v>9</v>
       </c>
@@ -602,8 +637,11 @@
       <c r="E11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
         <v>10</v>
       </c>
@@ -616,8 +654,11 @@
       <c r="E12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
         <v>11</v>
       </c>
@@ -630,8 +671,11 @@
       <c r="E13" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="13">
         <v>12</v>
       </c>
@@ -644,8 +688,11 @@
       <c r="E14" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="13">
         <v>13</v>
       </c>
@@ -658,8 +705,11 @@
       <c r="E15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" s="13">
         <v>14</v>
       </c>
@@ -672,8 +722,11 @@
       <c r="E16" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="13">
         <v>15</v>
       </c>
@@ -686,8 +739,11 @@
       <c r="E17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="13">
         <v>16</v>
       </c>
@@ -700,8 +756,11 @@
       <c r="E18" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="13">
         <v>17</v>
       </c>
@@ -714,8 +773,11 @@
       <c r="E19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="13">
         <v>18</v>
       </c>
@@ -728,8 +790,11 @@
       <c r="E20" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="13">
         <v>19</v>
       </c>
@@ -742,8 +807,11 @@
       <c r="E21" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="13">
         <v>20</v>
       </c>
@@ -756,8 +824,11 @@
       <c r="E22" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="13">
         <v>21</v>
       </c>
@@ -770,8 +841,11 @@
       <c r="E23" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -784,8 +858,11 @@
       <c r="E24" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="13">
         <v>23</v>
       </c>
@@ -798,8 +875,11 @@
       <c r="E25" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="13">
         <v>24</v>
       </c>
@@ -812,8 +892,11 @@
       <c r="E26" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="13">
         <v>25</v>
       </c>
@@ -826,8 +909,11 @@
       <c r="E27" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="13">
         <v>26</v>
       </c>
@@ -840,8 +926,11 @@
       <c r="E28" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="13">
         <v>27</v>
       </c>
@@ -854,8 +943,11 @@
       <c r="E29" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="13">
         <v>28</v>
       </c>
@@ -868,8 +960,11 @@
       <c r="E30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="13">
         <v>29</v>
       </c>
@@ -882,8 +977,11 @@
       <c r="E31" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B32" s="13">
         <v>30</v>
       </c>
@@ -896,8 +994,11 @@
       <c r="E32" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="13">
         <v>31</v>
       </c>
@@ -910,8 +1011,11 @@
       <c r="E33" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="13">
         <v>32</v>
       </c>
@@ -924,8 +1028,11 @@
       <c r="E34" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="13">
         <v>33</v>
       </c>
@@ -938,8 +1045,11 @@
       <c r="E35" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F35" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="13">
         <v>34</v>
       </c>
@@ -952,8 +1062,11 @@
       <c r="E36" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="13">
         <v>35</v>
       </c>
@@ -966,8 +1079,11 @@
       <c r="E37" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="13">
         <v>36</v>
       </c>
@@ -980,8 +1096,11 @@
       <c r="E38" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F38" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" s="13">
         <v>37</v>
       </c>
@@ -994,8 +1113,11 @@
       <c r="E39" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="13">
         <v>38</v>
       </c>
@@ -1008,8 +1130,11 @@
       <c r="E40" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F40" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" s="13">
         <v>39</v>
       </c>
@@ -1022,8 +1147,11 @@
       <c r="E41" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F41" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="13">
         <v>40</v>
       </c>
@@ -1036,22 +1164,28 @@
       <c r="E42" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F42" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B43" s="13">
         <v>41</v>
       </c>
-      <c r="C43" s="9">
-        <v>7243</v>
+      <c r="C43" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D43" s="4">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="E43" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F43" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B44" s="13">
         <v>42</v>
       </c>
@@ -1064,8 +1198,11 @@
       <c r="E44" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F44" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" s="13">
         <v>43</v>
       </c>
@@ -1078,8 +1215,11 @@
       <c r="E45" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F45" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" s="13">
         <v>44</v>
       </c>
@@ -1092,8 +1232,11 @@
       <c r="E46" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F46" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="13">
         <v>45</v>
       </c>
@@ -1106,50 +1249,68 @@
       <c r="E47" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F47" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" s="13">
         <v>46</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>6</v>
+      <c r="C48" s="9">
+        <v>7243</v>
       </c>
       <c r="D48" s="4">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="E48" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F48" s="14">
+        <v>1</v>
+      </c>
+      <c r="G48" s="9"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="15"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="13">
         <v>47</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D49" s="14">
+        <v>200</v>
       </c>
       <c r="E49" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F49" s="14">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" s="13">
         <v>48</v>
       </c>
-      <c r="C50" s="9">
-        <v>7217</v>
+      <c r="C50" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D50" s="4">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E50" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F50" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" s="13">
         <v>49</v>
       </c>
@@ -1162,78 +1323,96 @@
       <c r="E51" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F51" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="13">
         <v>50</v>
       </c>
       <c r="C52" s="9">
-        <v>7468</v>
+        <v>7217</v>
       </c>
       <c r="D52" s="4">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F52" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="13">
         <v>51</v>
       </c>
-      <c r="C53" s="9">
-        <v>7220</v>
+      <c r="C53" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D53" s="4">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="E53" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F53" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="13">
         <v>52</v>
       </c>
       <c r="C54" s="9">
-        <v>7493</v>
+        <v>7468</v>
       </c>
       <c r="D54" s="4">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E54" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F54" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" s="13">
         <v>53</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>6</v>
+      <c r="C55" s="9">
+        <v>7220</v>
       </c>
       <c r="D55" s="4">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="E55" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F55" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="13">
         <v>54</v>
       </c>
       <c r="C56" s="9">
-        <v>7846</v>
+        <v>7493</v>
       </c>
       <c r="D56" s="4">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F56" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="13">
         <v>55</v>
       </c>
@@ -1246,97 +1425,118 @@
       <c r="E57" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" s="13">
         <v>56</v>
       </c>
       <c r="C58" s="9">
-        <v>7221</v>
+        <v>7846</v>
       </c>
       <c r="D58" s="4">
-        <v>400</v>
+        <v>63</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F58" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="13">
         <v>57</v>
       </c>
-      <c r="C59" s="9">
-        <v>7222</v>
+      <c r="C59" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D59" s="4">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E59" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F59" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="13">
         <v>58</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>6</v>
+      <c r="C60" s="9">
+        <v>7221</v>
       </c>
       <c r="D60" s="4">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E60" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F60" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="13">
         <v>59</v>
       </c>
-      <c r="C61" s="11" t="s">
-        <v>5</v>
+      <c r="C61" s="9">
+        <v>7222</v>
       </c>
       <c r="D61" s="4">
-        <v>630</v>
+        <v>800</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F61" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="13">
         <v>60</v>
       </c>
-      <c r="C62" s="9">
-        <v>76102</v>
+      <c r="C62" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D62" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E62" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F62" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="13">
         <v>61</v>
       </c>
-      <c r="C63" s="9">
-        <v>7311</v>
+      <c r="C63" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="D63" s="4">
-        <v>100</v>
+        <v>630</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F63" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" s="13">
         <v>62</v>
       </c>
       <c r="C64" s="9">
-        <v>7206</v>
+        <v>76102</v>
       </c>
       <c r="D64" s="4">
         <v>100</v>
@@ -1344,36 +1544,45 @@
       <c r="E64" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F64" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B65" s="13">
         <v>63</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>6</v>
+      <c r="C65" s="9">
+        <v>7311</v>
       </c>
       <c r="D65" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E65" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F65" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B66" s="13">
         <v>64</v>
       </c>
       <c r="C66" s="9">
-        <v>7819</v>
+        <v>7206</v>
       </c>
       <c r="D66" s="4">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E66" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F66" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B67" s="13">
         <v>65</v>
       </c>
@@ -1386,22 +1595,28 @@
       <c r="E67" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F67" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B68" s="13">
         <v>66</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>6</v>
+      <c r="C68" s="9">
+        <v>7819</v>
       </c>
       <c r="D68" s="4">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E68" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F68" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B69" s="13">
         <v>67</v>
       </c>
@@ -1414,22 +1629,28 @@
       <c r="E69" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F69" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B70" s="13">
         <v>68</v>
       </c>
-      <c r="C70" s="9">
-        <v>7802</v>
+      <c r="C70" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D70" s="4">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E70" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F70" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B71" s="13">
         <v>69</v>
       </c>
@@ -1442,22 +1663,28 @@
       <c r="E71" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F71" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B72" s="13">
         <v>70</v>
       </c>
       <c r="C72" s="9">
-        <v>7250</v>
+        <v>7802</v>
       </c>
       <c r="D72" s="4">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="E72" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F72" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B73" s="13">
         <v>71</v>
       </c>
@@ -1470,64 +1697,79 @@
       <c r="E73" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F73" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B74" s="13">
         <v>72</v>
       </c>
       <c r="C74" s="9">
-        <v>7224</v>
+        <v>7250</v>
       </c>
       <c r="D74" s="4">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="E74" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F74" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B75" s="13">
         <v>73</v>
       </c>
-      <c r="C75" s="9">
-        <v>7811</v>
+      <c r="C75" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D75" s="4">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E75" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F75" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B76" s="13">
         <v>74</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>6</v>
+      <c r="C76" s="9">
+        <v>7224</v>
       </c>
       <c r="D76" s="4">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E76" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F76" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B77" s="13">
         <v>75</v>
       </c>
       <c r="C77" s="9">
-        <v>7807</v>
+        <v>7811</v>
       </c>
       <c r="D77" s="4">
-        <v>160</v>
+        <v>400</v>
       </c>
       <c r="E77" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F77" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B78" s="13">
         <v>76</v>
       </c>
@@ -1540,78 +1782,96 @@
       <c r="E78" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F78" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B79" s="13">
         <v>77</v>
       </c>
       <c r="C79" s="9">
-        <v>7228</v>
+        <v>7807</v>
       </c>
       <c r="D79" s="4">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="E79" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F79" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B80" s="13">
         <v>78</v>
       </c>
-      <c r="C80" s="9">
-        <v>72153</v>
+      <c r="C80" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D80" s="4">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="E80" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F80" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B81" s="13">
         <v>79</v>
       </c>
       <c r="C81" s="9">
-        <v>7240</v>
+        <v>7228</v>
       </c>
       <c r="D81" s="4">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="E81" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F81" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B82" s="13">
         <v>80</v>
       </c>
-      <c r="C82" s="9" t="s">
-        <v>6</v>
+      <c r="C82" s="9">
+        <v>72153</v>
       </c>
       <c r="D82" s="4">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="E82" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F82" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B83" s="13">
         <v>81</v>
       </c>
-      <c r="C83" s="9" t="s">
-        <v>6</v>
+      <c r="C83" s="9">
+        <v>7240</v>
       </c>
       <c r="D83" s="4">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="E83" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F83" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B84" s="13">
         <v>82</v>
       </c>
@@ -1624,78 +1884,96 @@
       <c r="E84" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F84" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B85" s="13">
         <v>83</v>
       </c>
-      <c r="C85" s="9">
-        <v>7302</v>
+      <c r="C85" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D85" s="4">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="E85" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F85" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B86" s="13">
         <v>84</v>
       </c>
-      <c r="C86" s="9">
-        <v>7223</v>
+      <c r="C86" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D86" s="4">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="E86" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F86" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B87" s="13">
         <v>85</v>
       </c>
       <c r="C87" s="9">
-        <v>7762</v>
+        <v>7302</v>
       </c>
       <c r="D87" s="4">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="E87" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F87" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B88" s="13">
         <v>86</v>
       </c>
-      <c r="C88" s="9" t="s">
-        <v>6</v>
+      <c r="C88" s="9">
+        <v>7223</v>
       </c>
       <c r="D88" s="4">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="E88" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F88" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" s="13">
         <v>87</v>
       </c>
       <c r="C89" s="9">
-        <v>7261</v>
+        <v>7762</v>
       </c>
       <c r="D89" s="4">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E89" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F89" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" s="13">
         <v>88</v>
       </c>
@@ -1708,13 +1986,16 @@
       <c r="E90" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F90" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B91" s="13">
         <v>89</v>
       </c>
       <c r="C91" s="9">
-        <v>72228</v>
+        <v>7261</v>
       </c>
       <c r="D91" s="4">
         <v>100</v>
@@ -1722,32 +2003,76 @@
       <c r="E91" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F91" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B92" s="13">
         <v>90</v>
       </c>
-      <c r="C92" s="10">
+      <c r="C92" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="4">
+        <v>0</v>
+      </c>
+      <c r="E92" s="5">
+        <v>0</v>
+      </c>
+      <c r="F92" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B93" s="13">
+        <v>91</v>
+      </c>
+      <c r="C93" s="9">
+        <v>72228</v>
+      </c>
+      <c r="D93" s="4">
+        <v>100</v>
+      </c>
+      <c r="E93" s="5">
+        <v>1</v>
+      </c>
+      <c r="F93" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B94" s="13">
+        <v>92</v>
+      </c>
+      <c r="C94" s="10">
         <v>7225</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D94" s="6">
         <v>800</v>
       </c>
-      <c r="E92" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C94" s="7" t="s">
+      <c r="E94" s="5">
+        <v>1</v>
+      </c>
+      <c r="F94" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C96" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D94">
-        <f>COUNTA(D3:D92)</f>
-        <v>90</v>
-      </c>
-      <c r="E94" s="2">
-        <f>SUM(E3:E92)</f>
-        <v>49</v>
+      <c r="D96">
+        <f>COUNTA(D3:D94)</f>
+        <v>92</v>
+      </c>
+      <c r="E96" s="2">
+        <f>SUM(E3:E94)</f>
+        <v>50</v>
+      </c>
+      <c r="F96">
+        <f>SUM(F3:F94)</f>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>